<commit_message>
finish analysis for adults & peds ed cohort
</commit_message>
<xml_diff>
--- a/scripts/antibiotic-susceptibility/sql/queries/aim_4/AIM4/csv_folder/Aim_4_Flowchart_Custom.xlsx
+++ b/scripts/antibiotic-susceptibility/sql/queries/aim_4/AIM4/csv_folder/Aim_4_Flowchart_Custom.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wenyuanchen/Desktop/Stanford/HealthRex/AIM4/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wenyuanchen/Desktop/Stanford/HealthRex/CDSS_aim4/scripts/antibiotic-susceptibility/sql/queries/aim_4/AIM4/csv_folder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1B3DF30-98BA-3340-BEB9-FD752DAA33AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC99980E-D7BC-9A4B-9E1C-D35E42118105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="8" xr2:uid="{2C2FEEC1-CE98-9E48-BF7C-57302DF83199}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{2C2FEEC1-CE98-9E48-BF7C-57302DF83199}"/>
   </bookViews>
   <sheets>
-    <sheet name="Overall" sheetId="1" r:id="rId1"/>
+    <sheet name="Step 6 (3)" sheetId="16" r:id="rId1"/>
     <sheet name="Step 1-2" sheetId="4" r:id="rId2"/>
     <sheet name="Step 3" sheetId="5" r:id="rId3"/>
     <sheet name="Step 3.2" sheetId="10" r:id="rId4"/>
@@ -22,6 +22,7 @@
     <sheet name="Step 4.2" sheetId="11" r:id="rId7"/>
     <sheet name="Step 5" sheetId="13" r:id="rId8"/>
     <sheet name="Step 6" sheetId="12" r:id="rId9"/>
+    <sheet name="Step 6 (2)" sheetId="15" r:id="rId10"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -44,10 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="41">
-  <si>
-    <t>N = 544,780</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="47">
   <si>
     <t xml:space="preserve">Adult Presumptive UTI Urine Culture Orders  </t>
   </si>
@@ -59,9 +57,6 @@
   </si>
   <si>
     <t>Excluded: Orders with Prior Order Within 14 Days</t>
-  </si>
-  <si>
-    <t>N = 121, 595</t>
   </si>
   <si>
     <t>N = 206,402</t>
@@ -101,9 +96,6 @@
   </si>
   <si>
     <t>Excluded: ED Orders with Non- Empirical Given Abx Med</t>
-  </si>
-  <si>
-    <t>Final ED Adult Presumptive UTI Urine Culture Order With Empirical Abx Med</t>
   </si>
   <si>
     <t>N =16,569</t>
@@ -320,21 +312,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">ED percentage of Given Abx Med                                               = 60,008/156,314                                                                                  </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="30"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>= 67.42%</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">ED percentage of Abx Med                                                                  = 79,916/156,314                                                                                    </t>
     </r>
     <r>
@@ -353,6 +330,48 @@
   </si>
   <si>
     <t>N =30,293</t>
+  </si>
+  <si>
+    <t>N = 3,662</t>
+  </si>
+  <si>
+    <t>N = 9,484</t>
+  </si>
+  <si>
+    <t>N =18,497</t>
+  </si>
+  <si>
+    <t>Number of Medications  to Be Evaluated</t>
+  </si>
+  <si>
+    <t>Final ED Adult Presumptive UTI Urine Culture Order With Empirical Given Abx Med</t>
+  </si>
+  <si>
+    <t>N = 480,007</t>
+  </si>
+  <si>
+    <t>N =480,007</t>
+  </si>
+  <si>
+    <t>Excluded: Orders Without Any Med</t>
+  </si>
+  <si>
+    <t>N = 56,822</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ED percentage of Given Abx Med                                               = 60,008/89,025                                                                                  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="30"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>= 89.77%</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -520,7 +539,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -549,9 +568,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -592,10 +608,10 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="12" name="Straight Arrow Connector 11">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01071736-B4BE-AF44-366C-86C151D3A913}"/>
+        <xdr:cNvPr id="2" name="Straight Arrow Connector 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFA3D951-8E2C-9242-8CEB-C3617869EBC5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -603,8 +619,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5934595" y="1160571"/>
-          <a:ext cx="0" cy="790318"/>
+          <a:off x="5949249" y="2130656"/>
+          <a:ext cx="0" cy="1337395"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -648,10 +664,10 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED338927-9DC2-9B9D-1F9F-12BCD020667D}"/>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A3F9E8D-44C6-D14D-86D8-CD3747A5A463}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -659,8 +675,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="5934595" y="1543538"/>
-          <a:ext cx="3697867" cy="12333"/>
+          <a:off x="5949249" y="3060700"/>
+          <a:ext cx="4855521" cy="12333"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -704,10 +720,10 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="16" name="Straight Arrow Connector 15">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B84C8F21-41DF-6943-94F6-AA1E4733A50D}"/>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7FE22AB-55EC-F34F-9FD6-D1243C8DB062}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -715,8 +731,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="6111561" y="2814823"/>
-          <a:ext cx="0" cy="1031841"/>
+          <a:off x="6114447" y="5096782"/>
+          <a:ext cx="0" cy="1832518"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -760,10 +776,10 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="18" name="Straight Arrow Connector 17">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A49E3B5-6A1F-5A40-95F4-3A616DFC003B}"/>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79754FB1-2600-EE41-BE64-69E7D670D662}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -771,8 +787,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8280787" y="7971922"/>
-          <a:ext cx="2475211" cy="0"/>
+          <a:off x="8287413" y="8513052"/>
+          <a:ext cx="2468585" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -816,10 +832,10 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="25" name="Straight Arrow Connector 24">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{738DFDFC-BD4D-F040-9477-65104D425F36}"/>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBBE8956-AF2C-0A4F-A091-94C1EC094CBA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -827,8 +843,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16388009" y="7835736"/>
-          <a:ext cx="1539832" cy="0"/>
+          <a:off x="16374718" y="8390992"/>
+          <a:ext cx="1538356" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -872,10 +888,10 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="27" name="Straight Arrow Connector 26">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52FED412-8C10-504E-8EAA-C11A4DF8685B}"/>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72B11F30-B695-B948-ACE5-A7EB15AB6EF4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -883,8 +899,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6183414" y="15855038"/>
-          <a:ext cx="4523663" cy="0"/>
+          <a:off x="6180653" y="14881555"/>
+          <a:ext cx="4526424" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -928,10 +944,10 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="30" name="Straight Arrow Connector 29">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A21DF2A-B0BD-D14A-983A-B49A78308DBB}"/>
+        <xdr:cNvPr id="8" name="Straight Arrow Connector 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3741599A-ACC4-4140-A46F-073B5159EE25}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -939,8 +955,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6129674" y="5475240"/>
-          <a:ext cx="0" cy="1694102"/>
+          <a:off x="6132560" y="9306599"/>
+          <a:ext cx="0" cy="2129366"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -984,10 +1000,10 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="31" name="Straight Arrow Connector 30">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1935E43B-0604-6743-90ED-BDE9F22F6520}"/>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{301EB79F-C105-BB4A-85DC-DB87DDD5EB4C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -995,8 +1011,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="6162386" y="6166419"/>
-          <a:ext cx="4160520" cy="0"/>
+          <a:off x="6165272" y="10138633"/>
+          <a:ext cx="4605020" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1040,10 +1056,10 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="42" name="Straight Arrow Connector 41">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACFE7582-CB20-1548-A09D-2878C9304C67}"/>
+        <xdr:cNvPr id="10" name="Straight Arrow Connector 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89A90790-74A6-9B4A-858F-65BA775DD781}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1051,8 +1067,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="6131214" y="9107366"/>
-          <a:ext cx="0" cy="603504"/>
+          <a:off x="6134100" y="14269916"/>
+          <a:ext cx="0" cy="1258709"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1096,10 +1112,10 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="63" name="Straight Arrow Connector 62">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0BC946F-6831-CD46-83D4-0A38893DCB26}"/>
+        <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{044DEF0F-79D9-A64A-8515-86D525FF4B1D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1107,8 +1123,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6183414" y="20879821"/>
-          <a:ext cx="4523663" cy="0"/>
+          <a:off x="6180653" y="19889221"/>
+          <a:ext cx="4526424" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1152,10 +1168,10 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="64" name="Straight Arrow Connector 63">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A9EA8CF-DB11-E949-AF0F-9B953985BAE0}"/>
+        <xdr:cNvPr id="12" name="Straight Arrow Connector 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C524B24-F073-DC44-96B2-27335EBA2607}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1163,8 +1179,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="6147496" y="10805082"/>
-          <a:ext cx="917" cy="1280160"/>
+          <a:off x="6136409" y="18881879"/>
+          <a:ext cx="917" cy="1755906"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1208,10 +1224,10 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="66" name="Straight Arrow Connector 65">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BC77CD7-0C6D-B342-A825-ADECE6645FDE}"/>
+        <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67174DD2-6427-4546-B18D-5884255E9CAB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1219,8 +1235,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6158242" y="26390494"/>
-          <a:ext cx="4530159" cy="0"/>
+          <a:off x="6161977" y="24971082"/>
+          <a:ext cx="4526424" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1264,10 +1280,10 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="67" name="Straight Arrow Connector 66">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6899E4EA-2DF3-AA4D-A4C7-EB4320AF84A7}"/>
+        <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5B1646F-7A15-AD44-82FC-9271ACDABFEC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1275,8 +1291,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6104867" y="13323059"/>
-          <a:ext cx="2309" cy="1280160"/>
+          <a:off x="6093780" y="24038432"/>
+          <a:ext cx="2309" cy="1735747"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1320,10 +1336,10 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="73" name="Straight Arrow Connector 72">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACD807AF-AD41-3447-9F76-05F5870C9160}"/>
+        <xdr:cNvPr id="15" name="Straight Arrow Connector 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3E634A7-1141-6C4D-9EE3-F393D8245D38}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1331,8 +1347,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6188591" y="30586865"/>
-          <a:ext cx="4538330" cy="0"/>
+          <a:off x="6180653" y="28631859"/>
+          <a:ext cx="4526424" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1376,10 +1392,10 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="74" name="Straight Arrow Connector 73">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E87A3365-2D78-FB4A-948D-A4F4E6295B52}"/>
+        <xdr:cNvPr id="16" name="Straight Arrow Connector 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B623E86C-3C9C-1C45-B2C5-DC2D9336C871}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1387,7 +1403,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6146800" y="30310016"/>
+          <a:off x="6108700" y="28087516"/>
           <a:ext cx="2309" cy="1355725"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -1432,10 +1448,10 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="75" name="Straight Arrow Connector 74">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B3714B9-B252-FC4A-B914-724F2E9338F3}"/>
+        <xdr:cNvPr id="17" name="Straight Arrow Connector 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F419A429-1C62-F946-933E-B89FD21E9859}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1443,8 +1459,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="3061988" y="34193922"/>
-          <a:ext cx="2668473" cy="731520"/>
+          <a:off x="3056466" y="32791400"/>
+          <a:ext cx="2671234" cy="755264"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1488,10 +1504,10 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="78" name="Straight Arrow Connector 77">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13D8E5A0-DE52-AB47-8CAC-4C8F7769AF60}"/>
+        <xdr:cNvPr id="18" name="Straight Arrow Connector 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E130CE1-585E-8845-8B23-E88B43D72B7B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1499,8 +1515,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6170728" y="34176988"/>
-          <a:ext cx="2862072" cy="731520"/>
+          <a:off x="6167967" y="32774466"/>
+          <a:ext cx="2871459" cy="755264"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1544,10 +1560,10 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="83" name="Straight Arrow Connector 82">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6AE992D3-3F7F-A54D-9A01-AC5A88D3CB92}"/>
+        <xdr:cNvPr id="19" name="Straight Arrow Connector 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{242BAC51-0DA5-9D4C-8EC3-54E0ED216191}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1555,8 +1571,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8252808" y="19344248"/>
-          <a:ext cx="2475211" cy="0"/>
+          <a:off x="8259434" y="18351991"/>
+          <a:ext cx="2468585" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1601,10 +1617,10 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="84" name="Straight Arrow Connector 83">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96C52EFF-D267-B84A-9EE4-247F7CA3282D}"/>
+        <xdr:cNvPr id="20" name="Straight Arrow Connector 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85042897-5C55-564C-97DA-A0DECC6C6BFF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1612,8 +1628,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8252808" y="24416799"/>
-          <a:ext cx="2475211" cy="0"/>
+          <a:off x="8259434" y="23738729"/>
+          <a:ext cx="2468585" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1658,10 +1674,10 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="87" name="Straight Arrow Connector 86">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9908588D-69DA-C045-9968-3DFDF87A3355}"/>
+        <xdr:cNvPr id="21" name="Straight Arrow Connector 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{064F7353-1B24-1240-8189-03F303C1FA4D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1669,8 +1685,1247 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6171406" y="5536406"/>
-          <a:ext cx="4538330" cy="0"/>
+          <a:off x="6163468" y="6083300"/>
+          <a:ext cx="4526424" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>360148</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>871941</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>360150</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Straight Arrow Connector 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E28EBD9-4B26-594F-AC70-C741A2F79FA3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="8178800" y="31970448"/>
+          <a:ext cx="2853141" cy="2"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1948749</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>85956</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1948749</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>407351</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="2" name="Straight Arrow Connector 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6AD327A4-E02E-D741-B5D6-7C5BD3AC3E91}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5949249" y="2130656"/>
+          <a:ext cx="0" cy="791295"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1948749</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>644770</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>12333</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0C052F0-D0D2-7C46-B40D-53AA762C5AD5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5949249" y="2514600"/>
+          <a:ext cx="4855521" cy="12333"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2113947</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>29482</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2113947</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>325300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13974ACC-A382-B043-9666-15ECF1988739}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6114447" y="4550682"/>
+          <a:ext cx="0" cy="1832518"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>108613</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1401052</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>595998</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1401052</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D51C0C9E-53EB-164D-8CD7-68348FEDC395}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8287413" y="7966952"/>
+          <a:ext cx="2468585" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>55218</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1278992</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>768074</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1278992</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB7631C3-6A8D-C349-8EA8-EDE25A527FDC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16400118" y="7844892"/>
+          <a:ext cx="1538356" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2180153</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>670255</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>547077</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>670255</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9220947-E4F8-FA4A-8DBE-C69A16882944}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6180653" y="14335455"/>
+          <a:ext cx="4526424" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2132060</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>149899</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2132060</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>285365</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Straight Arrow Connector 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46716B7D-638F-BD4C-AC9E-58674E175E7E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6132560" y="8760499"/>
+          <a:ext cx="0" cy="2129366"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2164772</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>4033</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>610292</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>4033</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9CF8894E-A0C8-0E48-827E-21474F339B65}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="6165272" y="9592533"/>
+          <a:ext cx="4605020" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2133600</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>58616</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2133600</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>301325</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Straight Arrow Connector 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A747A90-78B4-0E4B-9072-5EFAC53B6740}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6134100" y="13723816"/>
+          <a:ext cx="0" cy="1258709"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2180153</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>559821</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>547077</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>559821</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9AEC73D-9929-8243-9013-AE983B37EDF2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6180653" y="19343121"/>
+          <a:ext cx="4526424" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2135909</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>60479</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2136826</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>292385</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Straight Arrow Connector 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{498B468B-A07A-BA46-A8B5-04CF19E8128B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6136409" y="18335779"/>
+          <a:ext cx="917" cy="1755906"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2161477</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>523582</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>528401</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>523582</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83AB995D-90E3-AD45-9C3D-C2FFF38D4C8A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6161977" y="24424982"/>
+          <a:ext cx="4526424" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2093280</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>98932</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2095589</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>310679</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65C65819-A9B7-D14D-9935-ACA9873A7BE9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6093780" y="23492332"/>
+          <a:ext cx="2309" cy="1735747"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2180153</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>602959</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>547077</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>602959</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Straight Arrow Connector 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FA03902-3490-4947-89E4-213E9D1CB427}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6180653" y="28085759"/>
+          <a:ext cx="4526424" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2108200</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>58616</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2110509</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>398341</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Straight Arrow Connector 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6740847D-B2A6-4B47-8A9C-0E0E4C967F18}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6108700" y="27541416"/>
+          <a:ext cx="2309" cy="1355725"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1405466</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1727200</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>386964</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Straight Arrow Connector 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{598F0C10-460D-5F46-A032-F30CBD367BA2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3056466" y="31927800"/>
+          <a:ext cx="2671234" cy="729864"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2167467</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>135466</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>860626</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>370030</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Straight Arrow Connector 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{765D2F48-ADC9-2F41-A46E-32A7A95454D0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6167967" y="31910866"/>
+          <a:ext cx="2871459" cy="729864"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>80634</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>1067291</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>568019</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>1067291</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Straight Arrow Connector 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3A118E4-6C9A-8740-8A94-1771D3B3ED5A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8259434" y="17805891"/>
+          <a:ext cx="2468585" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>80634</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>1335929</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>568019</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>1335929</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Straight Arrow Connector 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA82314F-F3B8-E04D-8FBE-4921543F14B1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8259434" y="23192629"/>
+          <a:ext cx="2468585" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2162968</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>529892</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="Straight Arrow Connector 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BA1FE1D-814F-CE4C-B16F-2CA6F6772BB3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6163468" y="5537200"/>
+          <a:ext cx="4526424" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>360148</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>871941</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>360150</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Straight Arrow Connector 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D56899CD-8D95-BD48-ADCF-3C7497CD53CB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="8188657" y="31389849"/>
+          <a:ext cx="2862239" cy="2"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -6433,14 +7688,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC38303C-36AE-AA4C-B8CC-6B99D1FFC6A4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EC31857-08CB-C44F-B223-2362FE820B8D}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B1:J41"/>
   <sheetViews>
-    <sheetView zoomScale="50" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
+    <sheetView topLeftCell="A36" zoomScale="67" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="39" x14ac:dyDescent="0.45"/>
@@ -6450,10 +7705,9 @@
     <col min="4" max="4" width="54.83203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="26" style="1" customWidth="1"/>
     <col min="6" max="6" width="12" style="1" customWidth="1"/>
-    <col min="7" max="7" width="69.1640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="1"/>
-    <col min="9" max="9" width="10.83203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="65.1640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="68.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.83203125" style="1"/>
+    <col min="10" max="10" width="62.83203125" style="1" customWidth="1"/>
     <col min="11" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -6461,206 +7715,454 @@
     <row r="2" spans="2:10" ht="80" x14ac:dyDescent="0.45">
       <c r="B2" s="2"/>
       <c r="D2" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="2"/>
       <c r="D3" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" ht="37" customHeight="1" x14ac:dyDescent="0.45">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="80" x14ac:dyDescent="0.45">
       <c r="B4" s="2"/>
       <c r="G4" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="37" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B5" s="2"/>
       <c r="G5" s="4" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="80" x14ac:dyDescent="0.45">
       <c r="D6" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D7" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="80" x14ac:dyDescent="0.45">
       <c r="G8" s="3" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G9" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="40" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="11" spans="2:10" ht="160" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:10" ht="120" x14ac:dyDescent="0.45">
       <c r="D11" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D12" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="40" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="14" spans="2:10" ht="37" customHeight="1" x14ac:dyDescent="0.45">
       <c r="G14" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G15" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="4:7" ht="40" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="18" spans="4:7" ht="200" x14ac:dyDescent="0.45">
+    <row r="18" spans="4:7" ht="160" x14ac:dyDescent="0.45">
       <c r="D18" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="4:7" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D19" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="4:7" ht="80" x14ac:dyDescent="0.45">
       <c r="G20" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="4:7" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G21" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="4:7" ht="121" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D22" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="4:7" ht="121" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D23" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="4:7" ht="40" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="25" spans="4:7" ht="80" x14ac:dyDescent="0.45">
       <c r="G25" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="4:7" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G26" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="4:7" ht="121" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D27" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="4:7" ht="161" thickBot="1" x14ac:dyDescent="0.5">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="4:7" ht="121" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D28" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="4:7" ht="40" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="30" spans="4:7" ht="80" x14ac:dyDescent="0.45">
       <c r="G30" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="4:7" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G31" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="32" spans="4:7" ht="160" x14ac:dyDescent="0.45">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="4:7" ht="120" x14ac:dyDescent="0.45">
       <c r="D32" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="3:7" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D33" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34" spans="3:7" ht="80" x14ac:dyDescent="0.45">
       <c r="G34" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="3:7" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G35" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="36" spans="3:7" ht="160" x14ac:dyDescent="0.45">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="3:7" ht="161" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D36" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="37" spans="3:7" ht="56" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="D37" s="4" t="s">
-        <v>32</v>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="3:7" ht="81" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D37" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="3:7" ht="41" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G38" s="10" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="39" spans="3:7" ht="40" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="40" spans="3:7" ht="200" x14ac:dyDescent="0.45">
-      <c r="C40" s="3" t="s">
+    <row r="40" spans="3:7" ht="201" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C40" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E40" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E40" s="3" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="41" spans="3:7" ht="41" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C41" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>23</v>
+      <c r="C41" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="18" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup scale="19" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18F0F3B0-C45C-5044-8F02-D8AF86ACDF5D}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B1:J41"/>
+  <sheetViews>
+    <sheetView zoomScale="67" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="39" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="2" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="30.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="54.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="26" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12" style="1" customWidth="1"/>
+    <col min="7" max="7" width="68.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.83203125" style="1"/>
+    <col min="10" max="10" width="62.83203125" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10" ht="40" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="2" spans="2:10" ht="80" x14ac:dyDescent="0.45">
+      <c r="B2" s="2"/>
+      <c r="D2" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" ht="41" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B3" s="2"/>
+      <c r="D3" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="80" x14ac:dyDescent="0.45">
+      <c r="B4" s="2"/>
+      <c r="G4" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" ht="37" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B5" s="2"/>
+      <c r="G5" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" ht="80" x14ac:dyDescent="0.45">
+      <c r="D6" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" ht="41" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D7" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" ht="80" x14ac:dyDescent="0.45">
+      <c r="G8" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" ht="41" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G9" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" ht="40" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="11" spans="2:10" ht="120" x14ac:dyDescent="0.45">
+      <c r="D11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" ht="41" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" ht="40" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="14" spans="2:10" ht="37" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="G14" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" ht="41" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G15" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="4:7" ht="40" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="18" spans="4:7" ht="160" x14ac:dyDescent="0.45">
+      <c r="D18" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="4:7" ht="41" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D19" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="4:7" ht="80" x14ac:dyDescent="0.45">
+      <c r="G20" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="4:7" ht="41" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G21" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="4:7" ht="121" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D22" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="4:7" ht="121" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D23" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="4:7" ht="40" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="25" spans="4:7" ht="80" x14ac:dyDescent="0.45">
+      <c r="G25" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="4:7" ht="41" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G26" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="4:7" ht="121" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D27" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="4:7" ht="121" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D28" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="4:7" ht="40" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="30" spans="4:7" ht="80" x14ac:dyDescent="0.45">
+      <c r="G30" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="4:7" ht="41" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G31" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="4:7" ht="120" x14ac:dyDescent="0.45">
+      <c r="D32" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="3:7" ht="41" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D33" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="3:7" ht="80" x14ac:dyDescent="0.45">
+      <c r="G34" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="3:7" ht="41" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G35" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="3:7" ht="161" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D36" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="3:7" ht="81" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D37" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="3:7" ht="41" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G38" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="3:7" ht="40" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="40" spans="3:7" ht="201" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C40" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="3:7" ht="41" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C41" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="19" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -6672,8 +8174,8 @@
   </sheetPr>
   <dimension ref="B1:G7"/>
   <sheetViews>
-    <sheetView zoomScale="50" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" zoomScale="50" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="39" x14ac:dyDescent="0.45"/>
@@ -6683,7 +8185,7 @@
     <col min="4" max="4" width="54.83203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="26" style="1" customWidth="1"/>
     <col min="6" max="6" width="12" style="1" customWidth="1"/>
-    <col min="7" max="7" width="69.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="80.5" style="1" customWidth="1"/>
     <col min="8" max="9" width="10.83203125" style="1"/>
     <col min="10" max="10" width="49.5" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="10.83203125" style="1"/>
@@ -6693,35 +8195,35 @@
     <row r="2" spans="2:7" ht="80" x14ac:dyDescent="0.45">
       <c r="B2" s="2"/>
       <c r="D2" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="2:7" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="2"/>
       <c r="D3" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" ht="37" customHeight="1" x14ac:dyDescent="0.45">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="80" x14ac:dyDescent="0.45">
       <c r="B4" s="2"/>
       <c r="G4" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="37" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B5" s="2"/>
       <c r="G5" s="4" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="80" x14ac:dyDescent="0.45">
       <c r="D6" s="8" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D7" s="9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -6739,7 +8241,7 @@
   <dimension ref="B1:G12"/>
   <sheetViews>
     <sheetView zoomScale="41" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="39" x14ac:dyDescent="0.45"/>
@@ -6749,7 +8251,7 @@
     <col min="4" max="4" width="54.83203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="26" style="1" customWidth="1"/>
     <col min="6" max="6" width="12" style="1" customWidth="1"/>
-    <col min="7" max="7" width="69.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="103" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="10.83203125" style="1"/>
     <col min="10" max="10" width="49.5" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="10.83203125" style="1"/>
@@ -6759,56 +8261,56 @@
     <row r="2" spans="2:7" ht="80" x14ac:dyDescent="0.45">
       <c r="B2" s="2"/>
       <c r="D2" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="2:7" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="2"/>
       <c r="D3" s="4" t="s">
-        <v>0</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="37" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="2"/>
       <c r="G4" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="37" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B5" s="2"/>
       <c r="G5" s="4" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="80" x14ac:dyDescent="0.45">
       <c r="D6" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D7" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" ht="80" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="40" x14ac:dyDescent="0.45">
       <c r="G8" s="3" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G9" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="40" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="11" spans="2:7" ht="160" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:7" ht="120" x14ac:dyDescent="0.45">
       <c r="D11" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D12" s="9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -6826,7 +8328,7 @@
   <dimension ref="B1:G12"/>
   <sheetViews>
     <sheetView zoomScale="41" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="39" x14ac:dyDescent="0.45"/>
@@ -6846,62 +8348,62 @@
     <row r="2" spans="2:7" ht="80" x14ac:dyDescent="0.45">
       <c r="B2" s="2"/>
       <c r="D2" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="2:7" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="2"/>
       <c r="D3" s="4" t="s">
-        <v>0</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="37" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="2"/>
       <c r="G4" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="37" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B5" s="2"/>
       <c r="G5" s="4" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="80" x14ac:dyDescent="0.45">
       <c r="D6" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D7" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" ht="80" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="40" x14ac:dyDescent="0.45">
       <c r="G8" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G9" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="40" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="11" spans="2:7" ht="160" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:7" ht="120" x14ac:dyDescent="0.45">
       <c r="D11" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D12" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -6918,8 +8420,8 @@
   </sheetPr>
   <dimension ref="B1:J12"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="41" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView zoomScale="41" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="39" x14ac:dyDescent="0.45"/>
@@ -6939,72 +8441,68 @@
     <row r="2" spans="2:10" ht="80" x14ac:dyDescent="0.45">
       <c r="B2" s="2"/>
       <c r="D2" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="2"/>
       <c r="D3" s="4" t="s">
-        <v>0</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="2:10" ht="37" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="2"/>
       <c r="G4" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="37" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B5" s="2"/>
       <c r="G5" s="4" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="80" x14ac:dyDescent="0.45">
       <c r="D6" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D7" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="40" x14ac:dyDescent="0.45">
       <c r="G8" s="3" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G9" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" ht="40" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="J10" s="10"/>
-    </row>
-    <row r="11" spans="2:10" ht="160" x14ac:dyDescent="0.45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" ht="40" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="11" spans="2:10" ht="120" x14ac:dyDescent="0.45">
       <c r="D11" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I11" s="10"/>
+        <v>9</v>
+      </c>
       <c r="J11" s="8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D12" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="I12" s="10"/>
+        <v>24</v>
+      </c>
       <c r="J12" s="9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -7022,7 +8520,7 @@
   <dimension ref="B1:J37"/>
   <sheetViews>
     <sheetView topLeftCell="A6" zoomScale="50" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="39" x14ac:dyDescent="0.45"/>
@@ -7032,7 +8530,7 @@
     <col min="4" max="4" width="54.83203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="26" style="1" customWidth="1"/>
     <col min="6" max="6" width="12" style="1" customWidth="1"/>
-    <col min="7" max="7" width="69.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="109.83203125" style="1" customWidth="1"/>
     <col min="8" max="9" width="10.83203125" style="1"/>
     <col min="10" max="10" width="64.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="10.83203125" style="1"/>
@@ -7042,116 +8540,116 @@
     <row r="2" spans="2:10" ht="80" x14ac:dyDescent="0.45">
       <c r="B2" s="2"/>
       <c r="D2" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="2"/>
       <c r="D3" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" ht="37" customHeight="1" x14ac:dyDescent="0.45">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="2"/>
       <c r="G4" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="37" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B5" s="2"/>
       <c r="G5" s="4" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="80" x14ac:dyDescent="0.45">
       <c r="D6" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D7" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" ht="80" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" ht="40" x14ac:dyDescent="0.45">
       <c r="G8" s="3" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G9" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="40" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="11" spans="2:10" ht="120" x14ac:dyDescent="0.45">
       <c r="D11" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D12" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="40" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="14" spans="2:10" ht="37" customHeight="1" x14ac:dyDescent="0.45">
       <c r="G14" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G15" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="4:7" ht="40" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="18" spans="4:7" ht="201" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="18" spans="4:7" ht="161" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D18" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="4:7" ht="41" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="D19" s="11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="4:7" ht="80" x14ac:dyDescent="0.45">
+      <c r="D19" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="4:7" ht="40" x14ac:dyDescent="0.45">
       <c r="G20" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="4:7" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G21" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="4:7" ht="121" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D22" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="4:7" ht="121" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="D23" s="11" t="s">
-        <v>13</v>
+      <c r="D23" s="10" t="s">
+        <v>11</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -7170,7 +8668,7 @@
   <dimension ref="B1:J37"/>
   <sheetViews>
     <sheetView topLeftCell="A11" zoomScale="41" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="39" x14ac:dyDescent="0.45"/>
@@ -7180,7 +8678,7 @@
     <col min="4" max="4" width="54.83203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="26" style="1" customWidth="1"/>
     <col min="6" max="6" width="12" style="1" customWidth="1"/>
-    <col min="7" max="7" width="69.1640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="89.33203125" style="1" customWidth="1"/>
     <col min="8" max="9" width="10.83203125" style="1"/>
     <col min="10" max="10" width="62" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="10.83203125" style="1"/>
@@ -7190,143 +8688,143 @@
     <row r="2" spans="2:10" ht="80" x14ac:dyDescent="0.45">
       <c r="B2" s="2"/>
       <c r="D2" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="2"/>
       <c r="D3" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" ht="37" customHeight="1" x14ac:dyDescent="0.45">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="74" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="2"/>
       <c r="G4" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="37" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B5" s="2"/>
       <c r="G5" s="4" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="80" x14ac:dyDescent="0.45">
       <c r="D6" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D7" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" ht="80" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" ht="40" x14ac:dyDescent="0.45">
       <c r="G8" s="3" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G9" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="40" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="11" spans="2:10" ht="120" x14ac:dyDescent="0.45">
       <c r="D11" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D12" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="40" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="14" spans="2:10" ht="37" customHeight="1" x14ac:dyDescent="0.45">
       <c r="G14" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G15" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="4:7" ht="40" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="18" spans="4:7" ht="160" x14ac:dyDescent="0.45">
       <c r="D18" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="4:7" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D19" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="4:7" ht="80" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="4:7" ht="40" x14ac:dyDescent="0.45">
       <c r="G20" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="4:7" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G21" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="4:7" ht="121" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D22" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="4:7" ht="121" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D23" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="4:7" ht="40" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="25" spans="4:7" ht="80" x14ac:dyDescent="0.45">
       <c r="G25" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="4:7" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G26" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="4:7" ht="121" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D27" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="4:7" ht="161" thickBot="1" x14ac:dyDescent="0.5">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="4:7" ht="121" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D28" s="9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -7344,8 +8842,8 @@
   </sheetPr>
   <dimension ref="B1:J37"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="62" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView topLeftCell="A18" zoomScale="62" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="39" x14ac:dyDescent="0.45"/>
@@ -7365,164 +8863,164 @@
     <row r="2" spans="2:10" ht="80" x14ac:dyDescent="0.45">
       <c r="B2" s="2"/>
       <c r="D2" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="2"/>
       <c r="D3" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" ht="37" customHeight="1" x14ac:dyDescent="0.45">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="80" x14ac:dyDescent="0.45">
       <c r="B4" s="2"/>
       <c r="G4" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="37" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B5" s="2"/>
       <c r="G5" s="4" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="80" x14ac:dyDescent="0.45">
       <c r="D6" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D7" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="80" x14ac:dyDescent="0.45">
       <c r="G8" s="3" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G9" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="40" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="11" spans="2:10" ht="120" x14ac:dyDescent="0.45">
       <c r="D11" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D12" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="40" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="14" spans="2:10" ht="37" customHeight="1" x14ac:dyDescent="0.45">
       <c r="G14" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G15" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="4:7" ht="40" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="18" spans="4:7" ht="160" x14ac:dyDescent="0.45">
       <c r="D18" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="4:7" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D19" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="4:7" ht="80" x14ac:dyDescent="0.45">
       <c r="G20" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="4:7" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G21" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="4:7" ht="121" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D22" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="4:7" ht="121" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D23" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="4:7" ht="40" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="25" spans="4:7" ht="80" x14ac:dyDescent="0.45">
       <c r="G25" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="4:7" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G26" s="4" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="4:7" ht="121" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D27" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="4:7" ht="121" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D28" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="4:7" ht="40" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="30" spans="4:7" ht="80" x14ac:dyDescent="0.45">
       <c r="G30" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="4:7" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G31" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="4:7" ht="120" x14ac:dyDescent="0.45">
       <c r="D32" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="4:4" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D33" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="37" spans="4:4" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -7540,8 +9038,8 @@
   </sheetPr>
   <dimension ref="B1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="38" workbookViewId="0">
-      <selection activeCell="K44" sqref="K44"/>
+    <sheetView topLeftCell="B23" zoomScale="75" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="39" x14ac:dyDescent="0.45"/>
@@ -7551,7 +9049,7 @@
     <col min="4" max="4" width="54.83203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="26" style="1" customWidth="1"/>
     <col min="6" max="6" width="12" style="1" customWidth="1"/>
-    <col min="7" max="7" width="69.1640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="69" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="10.83203125" style="1"/>
     <col min="10" max="10" width="62.83203125" style="1" customWidth="1"/>
     <col min="11" max="16384" width="10.83203125" style="1"/>
@@ -7561,201 +9059,201 @@
     <row r="2" spans="2:10" ht="80" x14ac:dyDescent="0.45">
       <c r="B2" s="2"/>
       <c r="D2" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="2"/>
       <c r="D3" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" ht="37" customHeight="1" x14ac:dyDescent="0.45">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="80" x14ac:dyDescent="0.45">
       <c r="B4" s="2"/>
       <c r="G4" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="37" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B5" s="2"/>
       <c r="G5" s="4" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="80" x14ac:dyDescent="0.45">
       <c r="D6" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D7" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="80" x14ac:dyDescent="0.45">
       <c r="G8" s="3" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G9" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="40" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="11" spans="2:10" ht="120" x14ac:dyDescent="0.45">
       <c r="D11" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D12" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="40" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="14" spans="2:10" ht="37" customHeight="1" x14ac:dyDescent="0.45">
       <c r="G14" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G15" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="4:7" ht="40" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="18" spans="4:7" ht="160" x14ac:dyDescent="0.45">
       <c r="D18" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="4:7" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D19" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="4:7" ht="80" x14ac:dyDescent="0.45">
       <c r="G20" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="4:7" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G21" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="4:7" ht="121" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D22" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="4:7" ht="121" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D23" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="4:7" ht="40" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="25" spans="4:7" ht="80" x14ac:dyDescent="0.45">
       <c r="G25" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="4:7" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G26" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="4:7" ht="121" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D27" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="4:7" ht="121" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D28" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="4:7" ht="40" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="30" spans="4:7" ht="80" x14ac:dyDescent="0.45">
       <c r="G30" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="4:7" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G31" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="4:7" ht="120" x14ac:dyDescent="0.45">
       <c r="D32" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="3:7" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D33" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34" spans="3:7" ht="80" x14ac:dyDescent="0.45">
       <c r="G34" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="3:7" ht="41" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G35" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" spans="3:7" ht="161" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D36" s="3" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37" spans="3:7" ht="56" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="D37" s="11" t="s">
-        <v>32</v>
+      <c r="D37" s="10" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="39" spans="3:7" ht="40" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="40" spans="3:7" ht="201" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C40" s="12" t="s">
+      <c r="C40" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E40" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E40" s="3" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="41" spans="3:7" ht="41" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C41" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E41" s="11" t="s">
-        <v>23</v>
+      <c r="C41" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>